<commit_message>
Added a new testcase
Added a new testcase Itinerary
</commit_message>
<xml_diff>
--- a/POC/TestData/TestCasesData.xlsx
+++ b/POC/TestData/TestCasesData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>S.No</t>
   </si>
@@ -73,16 +73,25 @@
     <t>TC_007_Verify User is able to Click on Itinerary Link.</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
+    <t>21 Seconds</t>
+  </si>
+  <si>
+    <t>20 Seconds</t>
+  </si>
+  <si>
+    <t>19 Seconds</t>
+  </si>
+  <si>
+    <t>22 Seconds</t>
+  </si>
+  <si>
+    <t>17 Seconds</t>
+  </si>
+  <si>
     <t>16 Seconds</t>
-  </si>
-  <si>
-    <t>12 Seconds</t>
   </si>
 </sst>
 </file>
@@ -212,7 +221,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -247,7 +256,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -459,7 +468,7 @@
   <dimension ref="A1:H120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,16 +520,16 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1">
-        <v>0.76666666666666661</v>
+        <v>1.0011574074074074E-2</v>
       </c>
       <c r="G2" s="1">
-        <v>0.76680555555555552</v>
+        <v>1.0266203703703703E-2</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -537,16 +546,16 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1">
-        <v>0.76687500000000008</v>
+        <v>1.0277777777777778E-2</v>
       </c>
       <c r="G3" s="1">
-        <v>0.76706018518518515</v>
+        <v>1.0532407407407407E-2</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -560,10 +569,20 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="F4" s="1">
+        <v>1.0543981481481481E-2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1.0787037037037038E-2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -576,10 +595,20 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="F5" s="1">
+        <v>1.0798611111111111E-2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1.1018518518518518E-2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -592,10 +621,20 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="F6" s="1">
+        <v>1.1030092592592591E-2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1.1226851851851854E-2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -608,10 +647,20 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="F7" s="1">
+        <v>1.1238425925925928E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1.1469907407407408E-2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -624,10 +673,20 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="F8" s="1">
+        <v>1.1493055555555555E-2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1.1678240740740741E-2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F9" s="1"/>

</xml_diff>